<commit_message>
add selected and count-selected
</commit_message>
<xml_diff>
--- a/tests/003_DataSourceAndEmitColumns.xlsx
+++ b/tests/003_DataSourceAndEmitColumns.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t xml:space="preserve">Data Source</t>
   </si>
@@ -77,6 +77,21 @@
   </si>
   <si>
     <t xml:space="preserve">selected-at(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Danger Fever</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(fever)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Danger error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected-at(abc)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(fever</t>
   </si>
 </sst>
 </file>
@@ -188,21 +203,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3883928571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5982142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.9553571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.2767857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="23.4330357142857"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.5535714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3392857142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8035714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.3973214285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.5044642857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.8839285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="25.5133928571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.8616071428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="12.2857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -275,6 +290,39 @@
       </c>
       <c r="D6" s="2" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>